<commit_message>
files generation fixes & upd
</commit_message>
<xml_diff>
--- a/backend/data/Excel.xlsx
+++ b/backend/data/Excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Дата завдання</t>
   </si>
@@ -58,7 +58,13 @@
     <t>Коментар</t>
   </si>
   <si>
-    <t>default</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -88,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,33 +117,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="1" applyBorder="1" borderId="1"/>
-    <xf applyFont="1" fontId="0" applyBorder="1" borderId="2"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -207,9 +197,98 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+    <row r="2" spans="1:15">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>